<commit_message>
Working through check errors
</commit_message>
<xml_diff>
--- a/inst/check_notes_20210317.xlsx
+++ b/inst/check_notes_20210317.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gabrielodom/Documents/GitHub/coMethDMR/inst/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2243F415-15DB-0146-B0E0-6D5C1F4E9612}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{432E0190-4798-4046-A587-9C164C9E5F6E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{43E2E1ED-674D-F442-BDA2-47771752FD3D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="25">
   <si>
     <t xml:space="preserve">Type </t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>Add library() calls in vignette and package name to Suggests</t>
+  </si>
+  <si>
+    <t>importFrom dplyr n</t>
+  </si>
+  <si>
+    <t>importFrom rlang .data </t>
   </si>
 </sst>
 </file>
@@ -464,7 +470,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,6 +519,9 @@
       <c r="B4" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -520,6 +529,9 @@
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>